<commit_message>
Minor chnages in random graph
</commit_message>
<xml_diff>
--- a/4.1_Generating_a_random_signed_graph/performance_check/performance_check_Erdős_Rényi.xlsx
+++ b/4.1_Generating_a_random_signed_graph/performance_check/performance_check_Erdős_Rényi.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,10 +446,32 @@
         <v>50</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>8.414351851851851e-09</v>
+        <v>1.157407407407407e-08</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>2.236458333333333e-06</v>
+        <v>2.233796296296296e-06</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>2.164351851851852e-06</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>1.493055555555556e-09</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>2.094537037037037e-06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>